<commit_message>
Update Fett% to Fettinnhold
</commit_message>
<xml_diff>
--- a/Input_files_2020/NILU_template/Parameters_NILU_NIVA_2020.xlsx
+++ b/Input_files_2020/NILU_template/Parameters_NILU_NIVA_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\seksjon 212\Milkys2_pc\Input_files_2020\NILU_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CD6793-86C7-404C-A54E-7EC8A75136A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDAAC3-1DF2-4F2C-BA6C-432BF52277B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="-16635" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,9 +369,6 @@
     <t>Kvikksølv</t>
   </si>
   <si>
-    <t>Fett%</t>
-  </si>
-  <si>
     <t>FETT</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
     <t>Analysis: METALLER_ICPMS, METALLER_DGT_ICPMS eller METALLER_ICP_AES?</t>
   </si>
   <si>
-    <t>Finnes også "Fettinnhold" (også Analysis: FETT)</t>
-  </si>
-  <si>
     <t>Finnes også i DIOX_FURAN_PCBLIKE</t>
   </si>
   <si>
@@ -442,6 +436,12 @@
   </si>
   <si>
     <t>KVIKKSØLV</t>
+  </si>
+  <si>
+    <t>Fettinnhold</t>
+  </si>
+  <si>
+    <t>"Fett%" also used very uncommonly (only used for 12 blue mussels in some road runoff project, O 13326 - NCC SS)</t>
   </si>
 </sst>
 </file>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>83</v>
@@ -868,10 +868,10 @@
         <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>84</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -912,12 +912,12 @@
         <v>BDE17</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -930,12 +930,12 @@
         <v>BDE28</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -948,12 +948,12 @@
         <v>BDE47</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -966,12 +966,12 @@
         <v>BDE49</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -984,12 +984,12 @@
         <v>BDE66</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1002,12 +1002,12 @@
         <v>BDE71</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1020,12 +1020,12 @@
         <v>BDE77</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1038,12 +1038,12 @@
         <v>BDE85</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1056,12 +1056,12 @@
         <v>BDE99</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1074,12 +1074,12 @@
         <v>BDE100</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -1092,12 +1092,12 @@
         <v>BDE119</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -1110,12 +1110,12 @@
         <v>BDE126</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1128,12 +1128,12 @@
         <v>BDE138</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1146,12 +1146,12 @@
         <v>BDE153</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1164,12 +1164,12 @@
         <v>BDE154</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1182,12 +1182,12 @@
         <v>BDE156</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1200,12 +1200,12 @@
         <v>BDE183</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1218,12 +1218,12 @@
         <v>BDE184</v>
       </c>
       <c r="E20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1236,12 +1236,12 @@
         <v>BDE191</v>
       </c>
       <c r="E21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -1254,12 +1254,12 @@
         <v>BDE196</v>
       </c>
       <c r="E22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -1272,12 +1272,12 @@
         <v>BDE197</v>
       </c>
       <c r="E23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -1290,12 +1290,12 @@
         <v>BDE202</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -1308,12 +1308,12 @@
         <v>BDE206</v>
       </c>
       <c r="E25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -1326,12 +1326,12 @@
         <v>BDE207</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -1344,12 +1344,12 @@
         <v>BDE209</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -1364,7 +1364,7 @@
         <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>88</v>
@@ -1372,13 +1372,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
         <v>91</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
@@ -1424,12 +1424,12 @@
         <v>CB28</v>
       </c>
       <c r="G31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -1520,12 +1520,12 @@
         <v>CB52</v>
       </c>
       <c r="G37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
@@ -1601,12 +1601,12 @@
         <v>CB101</v>
       </c>
       <c r="G42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -1626,12 +1626,12 @@
         <v>CB105</v>
       </c>
       <c r="G43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -1651,12 +1651,12 @@
         <v>CB114</v>
       </c>
       <c r="G44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
@@ -1676,12 +1676,12 @@
         <v>CB118</v>
       </c>
       <c r="G45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
@@ -1716,12 +1716,12 @@
         <v>CB123</v>
       </c>
       <c r="G47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
@@ -1771,12 +1771,12 @@
         <v>CB138</v>
       </c>
       <c r="G50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
@@ -1826,12 +1826,12 @@
         <v>CB153</v>
       </c>
       <c r="G53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -1851,12 +1851,12 @@
         <v>CB156</v>
       </c>
       <c r="G54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
@@ -1876,12 +1876,12 @@
         <v>CB157</v>
       </c>
       <c r="G55" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -1901,12 +1901,12 @@
         <v>CB167</v>
       </c>
       <c r="G56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
         <v>55</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
         <v>57</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s">
         <v>58</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
         <v>59</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
         <v>60</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
         <v>62</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
         <v>63</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
@@ -2088,15 +2088,15 @@
         <v>95</v>
       </c>
       <c r="E68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" t="s">
         <v>67</v>
@@ -2105,15 +2105,15 @@
         <v>96</v>
       </c>
       <c r="E69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
         <v>68</v>
@@ -2122,15 +2122,15 @@
         <v>97</v>
       </c>
       <c r="E70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F70" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
@@ -2167,15 +2167,15 @@
         <v>102</v>
       </c>
       <c r="E73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B74" t="s">
         <v>72</v>
@@ -2184,12 +2184,12 @@
         <v>103</v>
       </c>
       <c r="E74" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B75" t="s">
         <v>73</v>
@@ -2198,12 +2198,12 @@
         <v>104</v>
       </c>
       <c r="E75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
         <v>74</v>
@@ -2212,12 +2212,12 @@
         <v>105</v>
       </c>
       <c r="E76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B77" t="s">
         <v>75</v>
@@ -2226,12 +2226,12 @@
         <v>106</v>
       </c>
       <c r="E77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B78" t="s">
         <v>76</v>
@@ -2240,12 +2240,12 @@
         <v>107</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B79" t="s">
         <v>77</v>
@@ -2254,12 +2254,12 @@
         <v>108</v>
       </c>
       <c r="E79" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
         <v>78</v>
@@ -2268,12 +2268,12 @@
         <v>109</v>
       </c>
       <c r="E80" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
         <v>79</v>
@@ -2282,12 +2282,12 @@
         <v>110</v>
       </c>
       <c r="E81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B82" t="s">
         <v>80</v>
@@ -2296,12 +2296,12 @@
         <v>111</v>
       </c>
       <c r="E82" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B83" t="s">
         <v>81</v>
@@ -2310,48 +2310,48 @@
         <v>112</v>
       </c>
       <c r="E83" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" t="s">
         <v>132</v>
-      </c>
-      <c r="B85" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B87" t="s">
         <v>82</v>
       </c>
       <c r="D87" t="s">
+        <v>136</v>
+      </c>
+      <c r="E87" t="s">
         <v>113</v>
       </c>
-      <c r="E87" t="s">
-        <v>114</v>
-      </c>
       <c r="G87" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>